<commit_message>
Code review and updates #13
</commit_message>
<xml_diff>
--- a/VSCode/Automatically Set Posting Period/Test/atdd.scenarios/ATDD Scenarios - Automatically Set Posting Period.xlsx
+++ b/VSCode/Automatically Set Posting Period/Test/atdd.scenarios/ATDD Scenarios - Automatically Set Posting Period.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvanv\source\repos\Test-Automation-Examples\VSCode\Automatically Set Posting Period\Test\atdd.scenarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvvugt\source\repos\Test-Automation-Examples\VSCode\Automatically Set Posting Period\Test\atdd.scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7865038B-5726-4AA5-9FBF-3BE404C3FEA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B3758D-77F8-43AF-BCFE-3C2DD5A8AD95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15990" xr2:uid="{DB99ADC0-1D36-4CB0-890F-ABAEDD9356F9}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{DB99ADC0-1D36-4CB0-890F-ABAEDD9356F9}"/>
   </bookViews>
   <sheets>
     <sheet name="ATDD Scenarios" sheetId="1" r:id="rId1"/>
@@ -99,12 +99,6 @@
     <t>Enable "Use Next Period" on Request Page</t>
   </si>
   <si>
-    <t>Set "Starting Date"  and "Ending Date" for current period</t>
-  </si>
-  <si>
-    <t>Set "Starting Date"  and "Ending Date" for next period</t>
-  </si>
-  <si>
     <t>UI testing using a RequestPageHandler</t>
   </si>
   <si>
@@ -232,6 +226,12 @@
   </si>
   <si>
     <t>Update G/L Setup with "Use Next Period" on Request Page disabled</t>
+  </si>
+  <si>
+    <t>Set "Starting Date" and "Ending Date" for next period</t>
+  </si>
+  <si>
+    <t>Set "Starting Date" and "Ending Date" for current period</t>
   </si>
 </sst>
 </file>
@@ -1437,7 +1437,7 @@
   <dimension ref="A1:L78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1488,7 +1488,7 @@
         <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>9</v>
@@ -1504,7 +1504,7 @@
       <c r="E2" s="13"/>
       <c r="F2" s="11"/>
       <c r="G2" s="21" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H2" s="14"/>
       <c r="I2" s="11" t="str">
@@ -1530,25 +1530,25 @@
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="3" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="H3" s="5">
         <v>1</v>
       </c>
       <c r="I3" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0001] Set "Starting Date"  and "Ending Date" for current period</v>
+        <v>[SCENARIO #0001] Set "Starting Date" and "Ending Date" for current period</v>
       </c>
       <c r="J3" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0001] Set "Starting Date"  and "Ending Date" for current period</v>
+        <v>//[SCENARIO #0001] Set "Starting Date" and "Ending Date" for current period</v>
       </c>
       <c r="K3" s="19" t="str">
         <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0001 'Set "Starting Date"  and "Ending Date" for current period' {</v>
+        <v>Scenario 0001 'Set "Starting Date" and "Ending Date" for current period' {</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1563,7 +1563,7 @@
         <v>16</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H4" s="5">
         <v>1</v>
@@ -1593,7 +1593,7 @@
         <v>16</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H5" s="5">
         <v>1</v>
@@ -1653,7 +1653,7 @@
         <v>18</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H7" s="5">
         <v>1</v>
@@ -1683,7 +1683,7 @@
         <v>18</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H8" s="5">
         <v>1</v>
@@ -1713,7 +1713,7 @@
         <v>18</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H9" s="5">
         <v>1</v>
@@ -1740,22 +1740,22 @@
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="3" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="H10" s="5">
         <v>2</v>
       </c>
       <c r="I10" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0002] Set "Starting Date"  and "Ending Date" for next period</v>
+        <v>[SCENARIO #0002] Set "Starting Date" and "Ending Date" for next period</v>
       </c>
       <c r="J10" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0002] Set "Starting Date"  and "Ending Date" for next period</v>
+        <v>//[SCENARIO #0002] Set "Starting Date" and "Ending Date" for next period</v>
       </c>
       <c r="K10" s="19" t="str">
         <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0002 'Set "Starting Date"  and "Ending Date" for next period' {</v>
+        <v>Scenario 0002 'Set "Starting Date" and "Ending Date" for next period' {</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1770,7 +1770,7 @@
         <v>16</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H11" s="5">
         <v>2</v>
@@ -1800,7 +1800,7 @@
         <v>16</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H12" s="5">
         <v>2</v>
@@ -1860,7 +1860,7 @@
         <v>18</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H14" s="5">
         <v>2</v>
@@ -1890,7 +1890,7 @@
         <v>18</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H15" s="5">
         <v>2</v>
@@ -1920,7 +1920,7 @@
         <v>18</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H16" s="5">
         <v>2</v>
@@ -1949,7 +1949,7 @@
         <v>10</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H17" s="5">
         <v>3</v>
@@ -1981,7 +1981,7 @@
         <v>16</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H18" s="5">
         <v>3</v>
@@ -2013,7 +2013,7 @@
         <v>17</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H19" s="5">
         <v>3</v>
@@ -2045,7 +2045,7 @@
         <v>18</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H20" s="5">
         <v>3</v>
@@ -2073,7 +2073,7 @@
       <c r="E21" s="13"/>
       <c r="F21" s="16"/>
       <c r="G21" s="21" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H21" s="14"/>
       <c r="I21" s="17" t="str">
@@ -2097,7 +2097,7 @@
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
       <c r="E22" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H22" s="5">
         <v>4</v>
@@ -2125,7 +2125,7 @@
         <v>16</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H23" s="5">
         <v>4</v>
@@ -2153,7 +2153,7 @@
         <v>16</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H24" s="5">
         <v>4</v>
@@ -2209,7 +2209,7 @@
         <v>17</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H26" s="5">
         <v>4</v>
@@ -2237,7 +2237,7 @@
         <v>18</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H27" s="5">
         <v>4</v>
@@ -2265,7 +2265,7 @@
         <v>18</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H28" s="5">
         <v>4</v>
@@ -2290,7 +2290,7 @@
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
       <c r="E29" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H29" s="5">
         <v>5</v>
@@ -2318,7 +2318,7 @@
         <v>16</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H30" s="5">
         <v>5</v>
@@ -2346,7 +2346,7 @@
         <v>16</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H31" s="5">
         <v>5</v>
@@ -2402,7 +2402,7 @@
         <v>17</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H33" s="5">
         <v>5</v>
@@ -2430,7 +2430,7 @@
         <v>18</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H34" s="5">
         <v>5</v>
@@ -2458,7 +2458,7 @@
         <v>18</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H35" s="5">
         <v>5</v>
@@ -2486,7 +2486,7 @@
       <c r="E36" s="13"/>
       <c r="F36" s="16"/>
       <c r="G36" s="21" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H36" s="14"/>
       <c r="I36" s="17" t="str">
@@ -2510,7 +2510,7 @@
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
       <c r="E37" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H37" s="5">
         <v>6</v>
@@ -2538,7 +2538,7 @@
         <v>16</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H38" s="5">
         <v>6</v>
@@ -2566,7 +2566,7 @@
         <v>16</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H39" s="5">
         <v>6</v>
@@ -2594,7 +2594,7 @@
         <v>16</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H40" s="5">
         <v>6</v>
@@ -2650,7 +2650,7 @@
         <v>17</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H42" s="5">
         <v>6</v>
@@ -2678,7 +2678,7 @@
         <v>18</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H43" s="5">
         <v>6</v>
@@ -2706,7 +2706,7 @@
         <v>18</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H44" s="5">
         <v>6</v>
@@ -2731,7 +2731,7 @@
       <c r="C45" s="10"/>
       <c r="D45" s="10"/>
       <c r="E45" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H45" s="5">
         <v>7</v>
@@ -2759,7 +2759,7 @@
         <v>16</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H46" s="5">
         <v>7</v>
@@ -2787,7 +2787,7 @@
         <v>16</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H47" s="5">
         <v>7</v>
@@ -2812,7 +2812,7 @@
         <v>16</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H48" s="5">
         <v>7</v>
@@ -2868,7 +2868,7 @@
         <v>17</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H50" s="5">
         <v>7</v>
@@ -2896,7 +2896,7 @@
         <v>18</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H51" s="5">
         <v>7</v>
@@ -2924,7 +2924,7 @@
         <v>18</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H52" s="5">
         <v>7</v>
@@ -2977,7 +2977,7 @@
         <v>16</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H54" s="5">
         <v>8</v>
@@ -3005,7 +3005,7 @@
         <v>16</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H55" s="5">
         <v>8</v>
@@ -3030,7 +3030,7 @@
         <v>16</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H56" s="5">
         <v>8</v>
@@ -3086,7 +3086,7 @@
         <v>17</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H58" s="5">
         <v>8</v>
@@ -3114,7 +3114,7 @@
         <v>18</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H59" s="5">
         <v>8</v>
@@ -3142,7 +3142,7 @@
         <v>18</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H60" s="5">
         <v>8</v>
@@ -3167,7 +3167,7 @@
       <c r="C61" s="10"/>
       <c r="D61" s="10"/>
       <c r="E61" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H61" s="5">
         <v>9</v>
@@ -3195,7 +3195,7 @@
         <v>16</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H62" s="5">
         <v>9</v>
@@ -3223,7 +3223,7 @@
         <v>16</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H63" s="5">
         <v>9</v>
@@ -3251,7 +3251,7 @@
         <v>16</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H64" s="5">
         <v>9</v>
@@ -3279,7 +3279,7 @@
         <v>16</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H65" s="5">
         <v>9</v>
@@ -3307,7 +3307,7 @@
         <v>16</v>
       </c>
       <c r="G66" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H66" s="5">
         <v>9</v>
@@ -3335,7 +3335,7 @@
         <v>16</v>
       </c>
       <c r="G67" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H67" s="5">
         <v>9</v>
@@ -3391,7 +3391,7 @@
         <v>17</v>
       </c>
       <c r="G69" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H69" s="5">
         <v>9</v>
@@ -3419,7 +3419,7 @@
         <v>18</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H70" s="5">
         <v>9</v>
@@ -3447,7 +3447,7 @@
         <v>18</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H71" s="5">
         <v>9</v>
@@ -3475,7 +3475,7 @@
         <v>18</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H72" s="5">
         <v>9</v>
@@ -3503,7 +3503,7 @@
         <v>18</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H73" s="5">
         <v>9</v>
@@ -3530,7 +3530,7 @@
       </c>
       <c r="D74" s="10"/>
       <c r="E74" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H74" s="5">
         <v>10</v>
@@ -3590,7 +3590,7 @@
         <v>17</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H76" s="5">
         <v>10</v>
@@ -3620,7 +3620,7 @@
         <v>18</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H77" s="5">
         <v>10</v>

</xml_diff>